<commit_message>
Update Shopping List 18.03.2025.xlsx
</commit_message>
<xml_diff>
--- a/Excel sheets/Shopping List 18.03.2025.xlsx
+++ b/Excel sheets/Shopping List 18.03.2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fotop\Documents\Semester Project 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fotop\Documents\Semester Project 2\GitHub Sem. Project 2\semester-project-2-\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ED5A35-7F26-4467-8C29-05AEA725EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DBBA8D-CD44-40CC-BA8C-D8F2F01E41C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{16E8840D-5B70-415D-8A66-4D39B7A66DDB}"/>
   </bookViews>
@@ -275,7 +275,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -312,6 +312,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="3" builtinId="30"/>
@@ -650,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FAF20B-D684-4DE0-825C-66A32388C60F}">
-  <dimension ref="C3:H20"/>
+  <dimension ref="C3:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -949,6 +950,9 @@
       <c r="H19" s="12"/>
     </row>
     <row r="20" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="D21" s="16"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H9" r:id="rId1" xr:uid="{EE5E5FF0-4CA5-4428-BA21-829952FAD4EB}"/>

</xml_diff>

<commit_message>
updated budget and made word document
</commit_message>
<xml_diff>
--- a/Excel sheets/Shopping List 18.03.2025.xlsx
+++ b/Excel sheets/Shopping List 18.03.2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\Desktop\semester project 2\semester-project-2-\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B608341E-E3E8-4131-BC51-2AB1D4D5289E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6AA821-A224-4634-A00E-E2BC864B35ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{16E8840D-5B70-415D-8A66-4D39B7A66DDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{16E8840D-5B70-415D-8A66-4D39B7A66DDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve">Shopping list </t>
   </si>
@@ -156,6 +156,18 @@
   </si>
   <si>
     <t>dafuq</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>3D printer filament</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>https://3deksperten.dk/products/3de-basic-pla-black-1-75mm-1kg</t>
   </si>
 </sst>
 </file>
@@ -660,7 +672,7 @@
   <dimension ref="C3:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,11 +973,24 @@
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="9"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="3"/>
+      <c r="C19" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="11">
+        <v>159.94999999999999</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="12" t="s">
@@ -973,8 +998,8 @@
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12">
-        <f>F6*G6+F7*G7+F8*G8+F9*G9+F10*G10+F11*G11+F12*G12+F13*G13+F14*G14+F15*G15+F16*G16+F17*G17+F18*G18</f>
-        <v>1571.55</v>
+        <f>F6*G6+F7*G7+F8*G8+F9*G9+F10*G10+F11*G11+F12*G12+F13*G13+F14*G14+F15*G15+F16*G16+F17*G17+F18*G18+F19*G19</f>
+        <v>1891.4499999999998</v>
       </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>

</xml_diff>